<commit_message>
New Api for Updating
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/ambient.app.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/ambient.app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE944AE1-5E17-DE4B-BC58-E8B3198980ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B458B38-6BA5-C141-BC80-0660EA34603E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70900" yWindow="-16800" windowWidth="35160" windowHeight="25040" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="45680" yWindow="-9760" windowWidth="41520" windowHeight="33480" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="145">
   <si>
     <t>key</t>
   </si>
@@ -458,6 +458,50 @@
   <si>
     <t>perm.app.module.read</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础数据/环境管理</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm.app.update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b20331d1-910f-4669-8c98-eec0eab35242</t>
+  </si>
+  <si>
+    <t>环境信息更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62e52251-6e19-4ec5-a7d3-cfdf2968d4ca</t>
+  </si>
+  <si>
+    <t>res.app.update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>848b0174-d492-4d51-a3cb-a3be7f650982</t>
+  </si>
+  <si>
+    <t>/api/app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.app.update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1169a3d-695f-4f81-a8f3-533ce592fa3e</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A3:I50"/>
+  <dimension ref="A3:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A42" sqref="A39:XFD42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1249,91 +1293,86 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
+    <row r="13" spans="1:9" s="21" customFormat="1">
+      <c r="A13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>101</v>
-      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>102</v>
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>108</v>
+      <c r="A18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>108</v>
@@ -1343,16 +1382,16 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>108</v>
@@ -1362,35 +1401,35 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>109</v>
@@ -1400,16 +1439,16 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>109</v>
@@ -1419,152 +1458,158 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="1" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C29" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="5" t="s">
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D31" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F31" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I31" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="14" t="str">
-        <f>A44</f>
-        <v>0e82ed16-91bf-4c41-b377-bd04d627c4d2</v>
-      </c>
-      <c r="C31" s="14" t="str">
-        <f>A18</f>
-        <v>b7dcf5e9-fc97-40f9-84c0-e35548b8f217</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G31" s="12" t="str">
-        <f>B18</f>
-        <v>单字典读取</v>
-      </c>
-      <c r="H31" s="12">
-        <v>2</v>
-      </c>
-      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="14" t="str">
-        <f>A45</f>
-        <v>48c1a5ad-a920-468d-820e-a994e629a83d</v>
+        <f t="shared" ref="B32:B39" si="0">A46</f>
+        <v>0e82ed16-91bf-4c41-b377-bd04d627c4d2</v>
       </c>
       <c r="C32" s="14" t="str">
-        <f>A19</f>
-        <v>f6f60dec-efad-4fc7-8715-e1cd58a100e5</v>
+        <f t="shared" ref="C32:C38" si="1">A19</f>
+        <v>b7dcf5e9-fc97-40f9-84c0-e35548b8f217</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G32" s="12" t="str">
-        <f>B19</f>
-        <v>单类字典读取</v>
+        <f t="shared" ref="G32:G38" si="2">B19</f>
+        <v>单字典读取</v>
       </c>
       <c r="H32" s="12">
         <v>2</v>
@@ -1573,28 +1618,28 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="14" t="str">
-        <f>A46</f>
-        <v>e94202f8-ea7e-4aeb-b8f8-5d0dae534490</v>
+        <f t="shared" si="0"/>
+        <v>48c1a5ad-a920-468d-820e-a994e629a83d</v>
       </c>
       <c r="C33" s="14" t="str">
-        <f>A20</f>
-        <v>b50b522b-8419-4ef5-869c-653d2af298d6</v>
+        <f t="shared" si="1"/>
+        <v>f6f60dec-efad-4fc7-8715-e1cd58a100e5</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G33" s="12" t="str">
-        <f>B20</f>
-        <v>多类字典读取</v>
+        <f t="shared" si="2"/>
+        <v>单类字典读取</v>
       </c>
       <c r="H33" s="12">
         <v>2</v>
@@ -1603,28 +1648,28 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="14" t="str">
-        <f>A47</f>
-        <v>a1d6e57c-3d50-438c-a1c4-229997d5945d</v>
+        <f t="shared" si="0"/>
+        <v>e94202f8-ea7e-4aeb-b8f8-5d0dae534490</v>
       </c>
       <c r="C34" s="14" t="str">
-        <f>A21</f>
-        <v>2c6f95c3-6105-4101-b693-4b783e081b5d</v>
+        <f t="shared" si="1"/>
+        <v>b50b522b-8419-4ef5-869c-653d2af298d6</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G34" s="12" t="str">
-        <f>B21</f>
-        <v>单类别读取</v>
+        <f t="shared" si="2"/>
+        <v>多类字典读取</v>
       </c>
       <c r="H34" s="12">
         <v>2</v>
@@ -1633,28 +1678,28 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="14" t="str">
-        <f>A48</f>
-        <v>09081a65-0367-47bb-bf96-dab26bc14399</v>
+        <f t="shared" si="0"/>
+        <v>a1d6e57c-3d50-438c-a1c4-229997d5945d</v>
       </c>
       <c r="C35" s="14" t="str">
-        <f>A22</f>
-        <v>7ccd1849-44a8-4002-ac2d-ffc6500370b5</v>
+        <f t="shared" si="1"/>
+        <v>2c6f95c3-6105-4101-b693-4b783e081b5d</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G35" s="12" t="str">
-        <f>B22</f>
-        <v>单类类别读取</v>
+        <f t="shared" si="2"/>
+        <v>单类别读取</v>
       </c>
       <c r="H35" s="12">
         <v>2</v>
@@ -1663,28 +1708,28 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="14" t="str">
-        <f>A49</f>
-        <v>8b12e4a2-eb23-41d7-ac93-1c6b5ef1b6ce</v>
+        <f t="shared" si="0"/>
+        <v>09081a65-0367-47bb-bf96-dab26bc14399</v>
       </c>
       <c r="C36" s="14" t="str">
-        <f>A23</f>
-        <v>baf05351-ed6f-4461-9824-36e171b03c78</v>
+        <f t="shared" si="1"/>
+        <v>7ccd1849-44a8-4002-ac2d-ffc6500370b5</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="G36" s="12" t="str">
-        <f>B23</f>
-        <v>多类类别读取</v>
+        <f t="shared" si="2"/>
+        <v>单类类别读取</v>
       </c>
       <c r="H36" s="12">
         <v>2</v>
@@ -1693,174 +1738,182 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="14" t="str">
-        <f>A50</f>
-        <v>f646b0db-c6ae-4691-b897-92a742388d05</v>
+        <f t="shared" si="0"/>
+        <v>8b12e4a2-eb23-41d7-ac93-1c6b5ef1b6ce</v>
       </c>
       <c r="C37" s="14" t="str">
-        <f>A24</f>
-        <v>b582539c-385d-4259-8374-1bd503555cf2</v>
+        <f t="shared" si="1"/>
+        <v>baf05351-ed6f-4461-9824-36e171b03c78</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G37" s="12" t="str">
-        <f>B24</f>
-        <v>模块信息读取</v>
+        <f t="shared" si="2"/>
+        <v>多类类别读取</v>
       </c>
       <c r="H37" s="12">
         <v>2</v>
       </c>
       <c r="I37" s="12"/>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
+    <row r="38" spans="1:9">
+      <c r="A38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>f646b0db-c6ae-4691-b897-92a742388d05</v>
+      </c>
+      <c r="C38" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>b582539c-385d-4259-8374-1bd503555cf2</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G38" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>模块信息读取</v>
+      </c>
+      <c r="H38" s="12">
+        <v>2</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>848b0174-d492-4d51-a3cb-a3be7f650982</v>
+      </c>
+      <c r="C39" s="14" t="str">
+        <f t="shared" ref="C39" si="3">A26</f>
+        <v>62e52251-6e19-4ec5-a7d3-cfdf2968d4ca</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="12" t="str">
+        <f t="shared" ref="G39" si="4">B26</f>
+        <v>环境信息更新</v>
+      </c>
+      <c r="H39" s="12">
+        <v>8</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C43" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="5" t="s">
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C44" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G44" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H44" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I44" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="7" t="s">
+    <row r="45" spans="1:9">
+      <c r="A45" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D45" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="H45" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I45" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="12" t="str">
-        <f>B18</f>
-        <v>单字典读取</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G44" s="12">
-        <v>2</v>
-      </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="12" t="str">
-        <f>B19</f>
-        <v>单类字典读取</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="12">
-        <v>2</v>
-      </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B46" s="12" t="str">
-        <f>B20</f>
-        <v>多类字典读取</v>
+        <f t="shared" ref="B46:B53" si="5">B19</f>
+        <v>单字典读取</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>108</v>
@@ -1876,20 +1929,20 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B47" s="12" t="str">
-        <f>B21</f>
-        <v>单类别读取</v>
+        <f t="shared" si="5"/>
+        <v>单类字典读取</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>105</v>
@@ -1902,20 +1955,20 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" s="12" t="str">
-        <f>B22</f>
-        <v>单类类别读取</v>
+        <f t="shared" si="5"/>
+        <v>多类字典读取</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>105</v>
@@ -1928,17 +1981,17 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" s="12" t="str">
-        <f>B23</f>
-        <v>多类类别读取</v>
+        <f t="shared" si="5"/>
+        <v>单类别读取</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>109</v>
@@ -1954,23 +2007,23 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="12" t="str">
-        <f>B24</f>
-        <v>模块信息读取</v>
+        <f t="shared" si="5"/>
+        <v>单类类别读取</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G50" s="12">
         <v>2</v>
@@ -1978,11 +2031,89 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
     </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>多类类别读取</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G51" s="12">
+        <v>2</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>模块信息读取</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" s="12">
+        <v>2</v>
+      </c>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>环境信息更新</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="12">
+        <v>8</v>
+      </c>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C43:I43"/>
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>